<commit_message>
Inicio crud de permisos de usuario
</commit_message>
<xml_diff>
--- a/src_php/db/formularios.xlsx
+++ b/src_php/db/formularios.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AppServ\www\temple_inventario\src_php\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76257B5A-F0B0-42C6-8A47-A0EC3AFA6201}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22836" windowHeight="10512"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22830" windowHeight="10515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="34">
   <si>
     <t>sis_unidad.php</t>
   </si>
@@ -123,13 +124,16 @@
   </si>
   <si>
     <t>acceso</t>
+  </si>
+  <si>
+    <t>form_formulario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +144,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -171,12 +183,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,27 +469,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="31.5546875" customWidth="1"/>
-    <col min="4" max="4" width="4.44140625" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -496,7 +509,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -513,7 +526,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -530,7 +543,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -547,7 +560,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
@@ -564,7 +577,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
@@ -581,7 +594,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
@@ -598,7 +611,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
@@ -615,7 +628,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
@@ -632,7 +645,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
@@ -649,7 +662,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
@@ -666,7 +679,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
@@ -683,7 +696,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
@@ -700,12 +713,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A16" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>29</v>
       </c>
@@ -724,6 +742,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modulo entradas y salidas
</commit_message>
<xml_diff>
--- a/src_php/db/formularios.xlsx
+++ b/src_php/db/formularios.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AppServ\www\temple_inventario\src_php\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76257B5A-F0B0-42C6-8A47-A0EC3AFA6201}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{74EE7DBA-56AD-4EB9-941E-38EA6AC2D93B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22830" windowHeight="10515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22830" windowHeight="10515" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="esquema archivos" sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="118">
   <si>
     <t>sis_unidad.php</t>
   </si>
@@ -127,13 +131,268 @@
   </si>
   <si>
     <t>form_formulario</t>
+  </si>
+  <si>
+    <t>Salario</t>
+  </si>
+  <si>
+    <t>dias</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>salario quincenal</t>
+  </si>
+  <si>
+    <t>salario diario</t>
+  </si>
+  <si>
+    <t>salario x hora</t>
+  </si>
+  <si>
+    <t>salario  mensual</t>
+  </si>
+  <si>
+    <t>1 mes</t>
+  </si>
+  <si>
+    <t>2 quincenal</t>
+  </si>
+  <si>
+    <t>30 diario</t>
+  </si>
+  <si>
+    <t>8 hora</t>
+  </si>
+  <si>
+    <t>INICIO SESION</t>
+  </si>
+  <si>
+    <t>GENERO TOKEN SALIDA</t>
+  </si>
+  <si>
+    <t>GENERO TOKEN ENTRADA</t>
+  </si>
+  <si>
+    <t>salidas</t>
+  </si>
+  <si>
+    <t>entradas</t>
+  </si>
+  <si>
+    <t>Revisar si token existe</t>
+  </si>
+  <si>
+    <t>Si no existe crearlo</t>
+  </si>
+  <si>
+    <t>Si existe recuperar encabezado</t>
+  </si>
+  <si>
+    <t>Si existe recuperar detalle</t>
+  </si>
+  <si>
+    <t>ir a tabla temporal</t>
+  </si>
+  <si>
+    <t>seleccionar concepto</t>
+  </si>
+  <si>
+    <t>opcional comentario</t>
+  </si>
+  <si>
+    <t>seleccionar sucursal</t>
+  </si>
+  <si>
+    <t>opcional codigo origen</t>
+  </si>
+  <si>
+    <t>Levantar modal, buscar producto</t>
+  </si>
+  <si>
+    <t>Puede elegir la unidad que descargara del producto</t>
+  </si>
+  <si>
+    <t>Permite guardar como borrador</t>
+  </si>
+  <si>
+    <t>Permite procesar</t>
+  </si>
+  <si>
+    <t>encabezado se guard en transacciones encabezado</t>
+  </si>
+  <si>
+    <t>detalle se guarda en transacciones detalle</t>
+  </si>
+  <si>
+    <t>cada detalle genera un registro en kardex</t>
+  </si>
+  <si>
+    <t>Puede eliminarse borrador</t>
+  </si>
+  <si>
+    <t>puede anularse procesado</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>php</t>
+  </si>
+  <si>
+    <t>Javascript</t>
+  </si>
+  <si>
+    <t>Componentes/</t>
+  </si>
+  <si>
+    <t>tabla.php</t>
+  </si>
+  <si>
+    <t>row</t>
+  </si>
+  <si>
+    <t>div col-sm-12</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>ESTE ES EL DETALLE</t>
+  </si>
+  <si>
+    <t>al final del index</t>
+  </si>
+  <si>
+    <t>en un script</t>
+  </si>
+  <si>
+    <t xml:space="preserve">con jquery </t>
+  </si>
+  <si>
+    <t>div.load/componente/tabla</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>div container</t>
+  </si>
+  <si>
+    <t>div buscador</t>
+  </si>
+  <si>
+    <t>div tabla que es detalle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">div modal abajo del </t>
+  </si>
+  <si>
+    <t>container pricipal</t>
+  </si>
+  <si>
+    <t>uno para nuevo</t>
+  </si>
+  <si>
+    <t>otro para edicion</t>
+  </si>
+  <si>
+    <t>cada modal tiene</t>
+  </si>
+  <si>
+    <t>tiene un boton con</t>
+  </si>
+  <si>
+    <t>data-target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">con el id del id para </t>
+  </si>
+  <si>
+    <t>abrirlo</t>
+  </si>
+  <si>
+    <t>modalNuevo</t>
+  </si>
+  <si>
+    <t>modalEdicion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En el body van </t>
+  </si>
+  <si>
+    <t>los campos a editar</t>
+  </si>
+  <si>
+    <t>obligatorio un id</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>conexión.php</t>
+  </si>
+  <si>
+    <t>variables de conexión</t>
+  </si>
+  <si>
+    <t>en el html de tabla</t>
+  </si>
+  <si>
+    <t>agregamos la consulta</t>
+  </si>
+  <si>
+    <t>en el cuerpo de la tabla</t>
+  </si>
+  <si>
+    <t>un nuevo script de jquery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y le agregamos una funcion </t>
+  </si>
+  <si>
+    <t>al clic de agregar</t>
+  </si>
+  <si>
+    <t>al final del index y</t>
+  </si>
+  <si>
+    <t>llamamos a funciones.js</t>
+  </si>
+  <si>
+    <t>funcion agregar_datos</t>
+  </si>
+  <si>
+    <t>dentro lleva un ajax</t>
+  </si>
+  <si>
+    <t>agregar_datos.php</t>
+  </si>
+  <si>
+    <t>esta funcion levanta la modal</t>
+  </si>
+  <si>
+    <t>y pone los datos a editarse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">actulaiza datos recupera </t>
+  </si>
+  <si>
+    <t>nuevamente los datos</t>
+  </si>
+  <si>
+    <t>y los envia al php</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,8 +415,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,8 +459,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -179,20 +486,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Título 2" xfId="2" builtinId="17"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -472,7 +814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -744,4 +1086,500 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873CCF80-C610-4ED5-80EE-982552473CB8}">
+  <dimension ref="F4:J12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="6:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="6:10" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F5" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="6:10" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F6" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="6:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="6:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="5">
+        <f>G4</f>
+        <v>300</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="6:10" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="5">
+        <f>G4/2</f>
+        <v>150</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="6:10" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="5">
+        <f>G4/30</f>
+        <v>10</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="6:10" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="5">
+        <f>G10/8</f>
+        <v>1.25</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" s="7">
+        <f>(G4/30)/8</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="12" spans="6:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249ABAAE-698B-4C6E-8CC8-AD8ACDD56183}">
+  <dimension ref="C3:F31"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="4" max="4" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0C756E5-08EC-4F73-AD92-5FD66CD6724C}">
+  <dimension ref="A1:F34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="30.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>105</v>
+      </c>
+      <c r="F18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{398BB7BE-7045-4C10-8393-6F04CDA14FB7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>